<commit_message>
Analysis of graph started, interesting results
</commit_message>
<xml_diff>
--- a/input/boosts.xlsx
+++ b/input/boosts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Scripts\ScratchPad\civ6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Leon\Scripts\Civ6Scripts\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{27CEF4B8-AFD5-4B36-99DD-024119BC8A76}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8998ADBD-6F67-46A2-8E60-033BB0ABC463}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="0" windowWidth="27870" windowHeight="12795" activeTab="3" xr2:uid="{02906B54-B3F8-4021-A19B-EF3C7ECABE5C}"/>
+    <workbookView xWindow="7440" yWindow="0" windowWidth="27870" windowHeight="12795" activeTab="4" xr2:uid="{02906B54-B3F8-4021-A19B-EF3C7ECABE5C}"/>
   </bookViews>
   <sheets>
     <sheet name="NodesOld" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="EraLookup" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'boost-edges'!$A$1:$C$242</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'boost-edges'!$A$1:$C$241</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'boost-nodes'!$A$1:$G$140</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">BoostsOld!$C$1:$J$114</definedName>
   </definedNames>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2545" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2542" uniqueCount="627">
   <si>
     <t>UNIT_BUILDER</t>
   </si>
@@ -7287,7 +7287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D7E711-A869-40B5-8321-E2CE58FD8C39}">
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -10589,10 +10589,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1554ACD1-5C2B-450B-8B98-E43CFCDB2298}">
-  <dimension ref="A1:C242"/>
+  <dimension ref="A1:C241"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124:XFD124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11956,10 +11956,10 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>403</v>
+        <v>305</v>
       </c>
       <c r="B124" t="s">
-        <v>448</v>
+        <v>480</v>
       </c>
       <c r="C124" t="s">
         <v>558</v>
@@ -11967,10 +11967,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>305</v>
+        <v>369</v>
       </c>
       <c r="B125" t="s">
-        <v>480</v>
+        <v>459</v>
       </c>
       <c r="C125" t="s">
         <v>558</v>
@@ -11978,10 +11978,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>369</v>
+        <v>308</v>
       </c>
       <c r="B126" t="s">
-        <v>459</v>
+        <v>479</v>
       </c>
       <c r="C126" t="s">
         <v>558</v>
@@ -11989,10 +11989,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>308</v>
+        <v>340</v>
       </c>
       <c r="B127" t="s">
-        <v>479</v>
+        <v>469</v>
       </c>
       <c r="C127" t="s">
         <v>558</v>
@@ -12000,10 +12000,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>340</v>
+        <v>107</v>
       </c>
       <c r="B128" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C128" t="s">
         <v>558</v>
@@ -12014,7 +12014,7 @@
         <v>107</v>
       </c>
       <c r="B129" t="s">
-        <v>470</v>
+        <v>28</v>
       </c>
       <c r="C129" t="s">
         <v>558</v>
@@ -12022,10 +12022,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>107</v>
+        <v>159</v>
       </c>
       <c r="B130" t="s">
-        <v>28</v>
+        <v>537</v>
       </c>
       <c r="C130" t="s">
         <v>558</v>
@@ -12033,10 +12033,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>159</v>
+        <v>313</v>
       </c>
       <c r="B131" t="s">
-        <v>537</v>
+        <v>477</v>
       </c>
       <c r="C131" t="s">
         <v>558</v>
@@ -12044,10 +12044,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B132" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C132" t="s">
         <v>558</v>
@@ -12055,10 +12055,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>311</v>
+        <v>194</v>
       </c>
       <c r="B133" t="s">
-        <v>478</v>
+        <v>524</v>
       </c>
       <c r="C133" t="s">
         <v>558</v>
@@ -12066,10 +12066,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>194</v>
+        <v>387</v>
       </c>
       <c r="B134" t="s">
-        <v>524</v>
+        <v>452</v>
       </c>
       <c r="C134" t="s">
         <v>558</v>
@@ -12077,10 +12077,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>387</v>
+        <v>316</v>
       </c>
       <c r="B135" t="s">
-        <v>452</v>
+        <v>476</v>
       </c>
       <c r="C135" t="s">
         <v>558</v>
@@ -12088,10 +12088,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>316</v>
+        <v>365</v>
       </c>
       <c r="B136" t="s">
-        <v>476</v>
+        <v>460</v>
       </c>
       <c r="C136" t="s">
         <v>558</v>
@@ -12099,10 +12099,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>365</v>
+        <v>210</v>
       </c>
       <c r="B137" t="s">
-        <v>460</v>
+        <v>517</v>
       </c>
       <c r="C137" t="s">
         <v>558</v>
@@ -12113,7 +12113,7 @@
         <v>210</v>
       </c>
       <c r="B138" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C138" t="s">
         <v>558</v>
@@ -12121,10 +12121,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>210</v>
+        <v>243</v>
       </c>
       <c r="B139" t="s">
-        <v>515</v>
+        <v>503</v>
       </c>
       <c r="C139" t="s">
         <v>558</v>
@@ -12132,10 +12132,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B140" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C140" t="s">
         <v>558</v>
@@ -12143,10 +12143,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>246</v>
+        <v>204</v>
       </c>
       <c r="B141" t="s">
-        <v>502</v>
+        <v>520</v>
       </c>
       <c r="C141" t="s">
         <v>558</v>
@@ -12154,10 +12154,10 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>204</v>
+        <v>357</v>
       </c>
       <c r="B142" t="s">
-        <v>520</v>
+        <v>463</v>
       </c>
       <c r="C142" t="s">
         <v>558</v>
@@ -12165,10 +12165,10 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>357</v>
+        <v>55</v>
       </c>
       <c r="B143" t="s">
-        <v>463</v>
+        <v>27</v>
       </c>
       <c r="C143" t="s">
         <v>558</v>
@@ -12176,10 +12176,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>55</v>
+        <v>227</v>
       </c>
       <c r="B144" t="s">
-        <v>27</v>
+        <v>510</v>
       </c>
       <c r="C144" t="s">
         <v>558</v>
@@ -12187,10 +12187,10 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="B145" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C145" t="s">
         <v>558</v>
@@ -12198,10 +12198,10 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>237</v>
+        <v>59</v>
       </c>
       <c r="B146" t="s">
-        <v>506</v>
+        <v>5</v>
       </c>
       <c r="C146" t="s">
         <v>558</v>
@@ -12209,10 +12209,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="B147" t="s">
-        <v>5</v>
+        <v>549</v>
       </c>
       <c r="C147" t="s">
         <v>558</v>
@@ -12220,10 +12220,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>121</v>
+        <v>220</v>
       </c>
       <c r="B148" t="s">
-        <v>549</v>
+        <v>513</v>
       </c>
       <c r="C148" t="s">
         <v>558</v>
@@ -12231,10 +12231,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>220</v>
+        <v>56</v>
       </c>
       <c r="B149" t="s">
-        <v>513</v>
+        <v>531</v>
       </c>
       <c r="C149" t="s">
         <v>558</v>
@@ -12242,10 +12242,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>56</v>
+        <v>322</v>
       </c>
       <c r="B150" t="s">
-        <v>531</v>
+        <v>474</v>
       </c>
       <c r="C150" t="s">
         <v>558</v>
@@ -12253,10 +12253,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>322</v>
+        <v>46</v>
       </c>
       <c r="B151" t="s">
-        <v>474</v>
+        <v>593</v>
       </c>
       <c r="C151" t="s">
         <v>558</v>
@@ -12267,7 +12267,7 @@
         <v>46</v>
       </c>
       <c r="B152" t="s">
-        <v>593</v>
+        <v>28</v>
       </c>
       <c r="C152" t="s">
         <v>558</v>
@@ -12275,10 +12275,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>46</v>
+        <v>148</v>
       </c>
       <c r="B153" t="s">
-        <v>28</v>
+        <v>540</v>
       </c>
       <c r="C153" t="s">
         <v>558</v>
@@ -12286,10 +12286,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>148</v>
+        <v>201</v>
       </c>
       <c r="B154" t="s">
-        <v>540</v>
+        <v>521</v>
       </c>
       <c r="C154" t="s">
         <v>558</v>
@@ -12297,10 +12297,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>201</v>
+        <v>108</v>
       </c>
       <c r="B155" t="s">
-        <v>521</v>
+        <v>542</v>
       </c>
       <c r="C155" t="s">
         <v>558</v>
@@ -12311,7 +12311,7 @@
         <v>108</v>
       </c>
       <c r="B156" t="s">
-        <v>542</v>
+        <v>29</v>
       </c>
       <c r="C156" t="s">
         <v>558</v>
@@ -12322,7 +12322,7 @@
         <v>108</v>
       </c>
       <c r="B157" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C157" t="s">
         <v>558</v>
@@ -12330,10 +12330,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>108</v>
+        <v>231</v>
       </c>
       <c r="B158" t="s">
-        <v>32</v>
+        <v>509</v>
       </c>
       <c r="C158" t="s">
         <v>558</v>
@@ -12341,10 +12341,10 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>231</v>
+        <v>110</v>
       </c>
       <c r="B159" t="s">
-        <v>509</v>
+        <v>451</v>
       </c>
       <c r="C159" t="s">
         <v>558</v>
@@ -12355,7 +12355,7 @@
         <v>110</v>
       </c>
       <c r="B160" t="s">
-        <v>451</v>
+        <v>508</v>
       </c>
       <c r="C160" t="s">
         <v>558</v>
@@ -12363,10 +12363,10 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B161" t="s">
-        <v>508</v>
+        <v>465</v>
       </c>
       <c r="C161" t="s">
         <v>558</v>
@@ -12374,10 +12374,10 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>109</v>
+        <v>399</v>
       </c>
       <c r="B162" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
       <c r="C162" t="s">
         <v>558</v>
@@ -12385,10 +12385,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>399</v>
+        <v>299</v>
       </c>
       <c r="B163" t="s">
-        <v>449</v>
+        <v>482</v>
       </c>
       <c r="C163" t="s">
         <v>558</v>
@@ -12396,10 +12396,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>299</v>
+        <v>225</v>
       </c>
       <c r="B164" t="s">
-        <v>482</v>
+        <v>511</v>
       </c>
       <c r="C164" t="s">
         <v>558</v>
@@ -12407,10 +12407,10 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="B165" t="s">
-        <v>511</v>
+        <v>525</v>
       </c>
       <c r="C165" t="s">
         <v>558</v>
@@ -12418,10 +12418,10 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>191</v>
+        <v>290</v>
       </c>
       <c r="B166" t="s">
-        <v>525</v>
+        <v>485</v>
       </c>
       <c r="C166" t="s">
         <v>558</v>
@@ -12429,10 +12429,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>290</v>
+        <v>111</v>
       </c>
       <c r="B167" t="s">
-        <v>485</v>
+        <v>462</v>
       </c>
       <c r="C167" t="s">
         <v>558</v>
@@ -12440,10 +12440,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>111</v>
+        <v>30</v>
       </c>
       <c r="B168" t="s">
-        <v>462</v>
+        <v>538</v>
       </c>
       <c r="C168" t="s">
         <v>558</v>
@@ -12451,10 +12451,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B169" t="s">
-        <v>538</v>
+        <v>522</v>
       </c>
       <c r="C169" t="s">
         <v>558</v>
@@ -12462,10 +12462,10 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B170" t="s">
-        <v>522</v>
+        <v>512</v>
       </c>
       <c r="C170" t="s">
         <v>558</v>
@@ -12473,10 +12473,10 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>19</v>
+        <v>581</v>
       </c>
       <c r="B171" t="s">
-        <v>512</v>
+        <v>551</v>
       </c>
       <c r="C171" t="s">
         <v>558</v>
@@ -12484,10 +12484,10 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>581</v>
+        <v>593</v>
       </c>
       <c r="B172" t="s">
-        <v>551</v>
+        <v>534</v>
       </c>
       <c r="C172" t="s">
         <v>558</v>
@@ -12495,10 +12495,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>593</v>
+        <v>582</v>
       </c>
       <c r="B173" t="s">
-        <v>534</v>
+        <v>25</v>
       </c>
       <c r="C173" t="s">
         <v>558</v>
@@ -12506,10 +12506,10 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B174" t="s">
-        <v>25</v>
+        <v>499</v>
       </c>
       <c r="C174" t="s">
         <v>558</v>
@@ -12517,10 +12517,10 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B175" t="s">
-        <v>499</v>
+        <v>527</v>
       </c>
       <c r="C175" t="s">
         <v>558</v>
@@ -12528,10 +12528,10 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B176" t="s">
-        <v>527</v>
+        <v>539</v>
       </c>
       <c r="C176" t="s">
         <v>558</v>
@@ -12539,10 +12539,10 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>585</v>
+        <v>38</v>
       </c>
       <c r="B177" t="s">
-        <v>539</v>
+        <v>488</v>
       </c>
       <c r="C177" t="s">
         <v>558</v>
@@ -12553,7 +12553,7 @@
         <v>38</v>
       </c>
       <c r="B178" t="s">
-        <v>488</v>
+        <v>1</v>
       </c>
       <c r="C178" t="s">
         <v>558</v>
@@ -12564,7 +12564,7 @@
         <v>38</v>
       </c>
       <c r="B179" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C179" t="s">
         <v>558</v>
@@ -12572,10 +12572,10 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B180" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C180" t="s">
         <v>558</v>
@@ -12583,10 +12583,10 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B181" t="s">
-        <v>32</v>
+        <v>498</v>
       </c>
       <c r="C181" t="s">
         <v>558</v>
@@ -12594,10 +12594,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B182" t="s">
-        <v>498</v>
+        <v>507</v>
       </c>
       <c r="C182" t="s">
         <v>558</v>
@@ -12605,10 +12605,10 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>47</v>
+        <v>212</v>
       </c>
       <c r="B183" t="s">
-        <v>507</v>
+        <v>455</v>
       </c>
       <c r="C183" t="s">
         <v>558</v>
@@ -12616,10 +12616,10 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>212</v>
+        <v>50</v>
       </c>
       <c r="B184" t="s">
-        <v>455</v>
+        <v>9</v>
       </c>
       <c r="C184" t="s">
         <v>558</v>
@@ -12627,10 +12627,10 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B185" t="s">
-        <v>9</v>
+        <v>583</v>
       </c>
       <c r="C185" t="s">
         <v>558</v>
@@ -12641,7 +12641,7 @@
         <v>58</v>
       </c>
       <c r="B186" t="s">
-        <v>583</v>
+        <v>16</v>
       </c>
       <c r="C186" t="s">
         <v>558</v>
@@ -12649,10 +12649,10 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B187" t="s">
-        <v>16</v>
+        <v>461</v>
       </c>
       <c r="C187" t="s">
         <v>558</v>
@@ -12660,10 +12660,10 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
       <c r="B188" t="s">
-        <v>461</v>
+        <v>586</v>
       </c>
       <c r="C188" t="s">
         <v>558</v>
@@ -12671,10 +12671,10 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>157</v>
+        <v>44</v>
       </c>
       <c r="B189" t="s">
-        <v>586</v>
+        <v>539</v>
       </c>
       <c r="C189" t="s">
         <v>558</v>
@@ -12685,7 +12685,7 @@
         <v>44</v>
       </c>
       <c r="B190" t="s">
-        <v>539</v>
+        <v>33</v>
       </c>
       <c r="C190" t="s">
         <v>558</v>
@@ -12693,10 +12693,10 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>44</v>
+        <v>247</v>
       </c>
       <c r="B191" t="s">
-        <v>33</v>
+        <v>446</v>
       </c>
       <c r="C191" t="s">
         <v>558</v>
@@ -12704,10 +12704,10 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>247</v>
+        <v>39</v>
       </c>
       <c r="B192" t="s">
-        <v>446</v>
+        <v>30</v>
       </c>
       <c r="C192" t="s">
         <v>558</v>
@@ -12718,7 +12718,7 @@
         <v>39</v>
       </c>
       <c r="B193" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C193" t="s">
         <v>558</v>
@@ -12726,10 +12726,10 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B194" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C194" t="s">
         <v>558</v>
@@ -12737,10 +12737,10 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>54</v>
+        <v>205</v>
       </c>
       <c r="B195" t="s">
-        <v>20</v>
+        <v>582</v>
       </c>
       <c r="C195" t="s">
         <v>558</v>
@@ -12748,10 +12748,10 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>205</v>
+        <v>42</v>
       </c>
       <c r="B196" t="s">
-        <v>582</v>
+        <v>19</v>
       </c>
       <c r="C196" t="s">
         <v>558</v>
@@ -12762,7 +12762,7 @@
         <v>42</v>
       </c>
       <c r="B197" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C197" t="s">
         <v>558</v>
@@ -12770,10 +12770,10 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B198" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C198" t="s">
         <v>558</v>
@@ -12781,10 +12781,10 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
       <c r="B199" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C199" t="s">
         <v>558</v>
@@ -12795,7 +12795,7 @@
         <v>93</v>
       </c>
       <c r="B200" t="s">
-        <v>30</v>
+        <v>584</v>
       </c>
       <c r="C200" t="s">
         <v>558</v>
@@ -12803,10 +12803,10 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="B201" t="s">
-        <v>584</v>
+        <v>505</v>
       </c>
       <c r="C201" t="s">
         <v>558</v>
@@ -12817,7 +12817,7 @@
         <v>43</v>
       </c>
       <c r="B202" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="C202" t="s">
         <v>558</v>
@@ -12828,7 +12828,7 @@
         <v>43</v>
       </c>
       <c r="B203" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="C203" t="s">
         <v>558</v>
@@ -12839,7 +12839,7 @@
         <v>43</v>
       </c>
       <c r="B204" t="s">
-        <v>493</v>
+        <v>551</v>
       </c>
       <c r="C204" t="s">
         <v>558</v>
@@ -12850,7 +12850,7 @@
         <v>43</v>
       </c>
       <c r="B205" t="s">
-        <v>551</v>
+        <v>527</v>
       </c>
       <c r="C205" t="s">
         <v>558</v>
@@ -12861,7 +12861,7 @@
         <v>43</v>
       </c>
       <c r="B206" t="s">
-        <v>527</v>
+        <v>495</v>
       </c>
       <c r="C206" t="s">
         <v>558</v>
@@ -12869,10 +12869,10 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>43</v>
+        <v>147</v>
       </c>
       <c r="B207" t="s">
-        <v>495</v>
+        <v>481</v>
       </c>
       <c r="C207" t="s">
         <v>558</v>
@@ -12880,10 +12880,10 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="B208" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="C208" t="s">
         <v>558</v>
@@ -12894,7 +12894,7 @@
         <v>171</v>
       </c>
       <c r="B209" t="s">
-        <v>475</v>
+        <v>581</v>
       </c>
       <c r="C209" t="s">
         <v>558</v>
@@ -12902,10 +12902,10 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>171</v>
+        <v>40</v>
       </c>
       <c r="B210" t="s">
-        <v>581</v>
+        <v>496</v>
       </c>
       <c r="C210" t="s">
         <v>558</v>
@@ -12916,7 +12916,7 @@
         <v>40</v>
       </c>
       <c r="B211" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="C211" t="s">
         <v>558</v>
@@ -12924,10 +12924,10 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B212" t="s">
-        <v>500</v>
+        <v>3</v>
       </c>
       <c r="C212" t="s">
         <v>558</v>
@@ -12935,10 +12935,10 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B213" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C213" t="s">
         <v>558</v>
@@ -12946,10 +12946,10 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B214" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C214" t="s">
         <v>558</v>
@@ -12957,10 +12957,10 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>52</v>
+        <v>176</v>
       </c>
       <c r="B215" t="s">
-        <v>25</v>
+        <v>585</v>
       </c>
       <c r="C215" t="s">
         <v>558</v>
@@ -12968,10 +12968,10 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>176</v>
+        <v>53</v>
       </c>
       <c r="B216" t="s">
-        <v>585</v>
+        <v>24</v>
       </c>
       <c r="C216" t="s">
         <v>558</v>
@@ -12979,10 +12979,10 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>53</v>
+        <v>142</v>
       </c>
       <c r="B217" t="s">
-        <v>24</v>
+        <v>487</v>
       </c>
       <c r="C217" t="s">
         <v>558</v>
@@ -12990,10 +12990,10 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>142</v>
+        <v>264</v>
       </c>
       <c r="B218" t="s">
-        <v>487</v>
+        <v>507</v>
       </c>
       <c r="C218" t="s">
         <v>558</v>
@@ -13001,10 +13001,10 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>264</v>
+        <v>28</v>
       </c>
       <c r="B219" t="s">
-        <v>507</v>
+        <v>534</v>
       </c>
       <c r="C219" t="s">
         <v>558</v>
@@ -13012,10 +13012,10 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B220" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C220" t="s">
         <v>558</v>
@@ -13023,10 +13023,10 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B221" t="s">
-        <v>535</v>
+        <v>519</v>
       </c>
       <c r="C221" t="s">
         <v>558</v>
@@ -13034,10 +13034,10 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B222" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C222" t="s">
         <v>558</v>
@@ -13045,10 +13045,10 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B223" t="s">
-        <v>518</v>
+        <v>472</v>
       </c>
       <c r="C223" t="s">
         <v>558</v>
@@ -13056,10 +13056,10 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B224" t="s">
-        <v>472</v>
+        <v>545</v>
       </c>
       <c r="C224" t="s">
         <v>558</v>
@@ -13067,10 +13067,10 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B225" t="s">
-        <v>545</v>
+        <v>530</v>
       </c>
       <c r="C225" t="s">
         <v>558</v>
@@ -13078,10 +13078,10 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B226" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="C226" t="s">
         <v>558</v>
@@ -13089,10 +13089,10 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="B227" t="s">
-        <v>523</v>
+        <v>30</v>
       </c>
       <c r="C227" t="s">
         <v>558</v>
@@ -13103,7 +13103,7 @@
         <v>95</v>
       </c>
       <c r="B228" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C228" t="s">
         <v>558</v>
@@ -13111,10 +13111,10 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="B229" t="s">
-        <v>23</v>
+        <v>529</v>
       </c>
       <c r="C229" t="s">
         <v>558</v>
@@ -13125,7 +13125,7 @@
         <v>20</v>
       </c>
       <c r="B230" t="s">
-        <v>529</v>
+        <v>516</v>
       </c>
       <c r="C230" t="s">
         <v>558</v>
@@ -13133,10 +13133,10 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B231" t="s">
-        <v>516</v>
+        <v>532</v>
       </c>
       <c r="C231" t="s">
         <v>558</v>
@@ -13144,10 +13144,10 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="B232" t="s">
-        <v>532</v>
+        <v>453</v>
       </c>
       <c r="C232" t="s">
         <v>558</v>
@@ -13155,10 +13155,10 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B233" t="s">
-        <v>453</v>
+        <v>441</v>
       </c>
       <c r="C233" t="s">
         <v>558</v>
@@ -13169,7 +13169,7 @@
         <v>1</v>
       </c>
       <c r="B234" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="C234" t="s">
         <v>558</v>
@@ -13180,7 +13180,7 @@
         <v>1</v>
       </c>
       <c r="B235" t="s">
-        <v>447</v>
+        <v>489</v>
       </c>
       <c r="C235" t="s">
         <v>558</v>
@@ -13191,7 +13191,7 @@
         <v>1</v>
       </c>
       <c r="B236" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="C236" t="s">
         <v>558</v>
@@ -13199,10 +13199,10 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B237" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C237" t="s">
         <v>558</v>
@@ -13210,10 +13210,10 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B238" t="s">
-        <v>491</v>
+        <v>504</v>
       </c>
       <c r="C238" t="s">
         <v>558</v>
@@ -13221,10 +13221,10 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B239" t="s">
-        <v>504</v>
+        <v>547</v>
       </c>
       <c r="C239" t="s">
         <v>558</v>
@@ -13232,10 +13232,10 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B240" t="s">
-        <v>547</v>
+        <v>458</v>
       </c>
       <c r="C240" t="s">
         <v>558</v>
@@ -13246,33 +13246,22 @@
         <v>5</v>
       </c>
       <c r="B241" t="s">
-        <v>458</v>
+        <v>497</v>
       </c>
       <c r="C241" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
-        <v>5</v>
-      </c>
-      <c r="B242" t="s">
-        <v>497</v>
-      </c>
-      <c r="C242" t="s">
-        <v>558</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:C242" xr:uid="{96C1B2F8-F8A0-469A-8041-02863A68134F}">
-    <sortState ref="A2:C242">
-      <sortCondition ref="A2:A242"/>
-      <sortCondition ref="B2:B242"/>
+  <autoFilter ref="A1:C241" xr:uid="{96C1B2F8-F8A0-469A-8041-02863A68134F}">
+    <sortState ref="A2:C241">
+      <sortCondition ref="A2:A241"/>
+      <sortCondition ref="B2:B241"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:C241">
-    <sortCondition ref="A2:A241"/>
-    <sortCondition ref="B2:B241"/>
+  <sortState ref="A2:C240">
+    <sortCondition ref="A2:A240"/>
+    <sortCondition ref="B2:B240"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>